<commit_message>
Se actualizan las cosas faltantes. Se verifica la placa Poncho EDUCIAA.
</commit_message>
<xml_diff>
--- a/Utilidades/cosas_faltantes/2019/Faltantes.xlsx
+++ b/Utilidades/cosas_faltantes/2019/Faltantes.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF21167-7333-42D8-BDC2-691DD9278B23}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A22A6392-DCF2-4787-8E3F-B67140CFFA79}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
   <si>
     <t>PUNCH LIST 2019</t>
   </si>
@@ -115,7 +115,10 @@
     <t>FINALIZADO</t>
   </si>
   <si>
-    <t>No se va a hacer.</t>
+    <t>Ahora hay que hacerlo.</t>
+  </si>
+  <si>
+    <t>Afinar tiempos y posibilidad de juntar datos más rápidamente.</t>
   </si>
 </sst>
 </file>
@@ -284,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -350,6 +353,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -691,8 +695,8 @@
   <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,11 +754,11 @@
         <v>4</v>
       </c>
       <c r="B5" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="10"/>
-      <c r="D5" s="18">
-        <v>43518</v>
+      <c r="D5" s="19" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -774,13 +778,13 @@
         <v>16</v>
       </c>
       <c r="B7" s="14">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="18">
-        <v>43511</v>
+      <c r="D7" s="19" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -793,16 +797,14 @@
       <c r="C8" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="19" t="s">
-        <v>31</v>
-      </c>
+      <c r="D8" s="27"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="14">
-        <v>0.2</v>
+        <v>0.7</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="2"/>
@@ -836,7 +838,7 @@
         <v>23</v>
       </c>
       <c r="B12" s="14">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>26</v>
@@ -880,20 +882,24 @@
         <v>6</v>
       </c>
       <c r="B18" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="9"/>
-      <c r="D18" s="3"/>
+      <c r="D18" s="19" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B19" s="14">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="C19" s="10"/>
-      <c r="D19" s="2"/>
+      <c r="D19" s="19" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
@@ -1012,10 +1018,12 @@
         <v>28</v>
       </c>
       <c r="B34" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C34" s="10"/>
-      <c r="D34" s="2"/>
+      <c r="D34" s="19" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="10"/>
@@ -1042,9 +1050,11 @@
         <v>15</v>
       </c>
       <c r="B38" s="13">
-        <v>0.9</v>
-      </c>
-      <c r="C38" s="9"/>
+        <v>0.8</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>33</v>
+      </c>
       <c r="D38" s="3"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1052,10 +1062,12 @@
         <v>29</v>
       </c>
       <c r="B39" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C39" s="10"/>
-      <c r="D39" s="2"/>
+      <c r="D39" s="19" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>

</xml_diff>